<commit_message>
Text and picture additions
</commit_message>
<xml_diff>
--- a/wwwroot/Data/BooksDB.xlsx
+++ b/wwwroot/Data/BooksDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgreen3\Desktop\FunWithBrandt\wwwroot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0485C3-DD42-4DB5-91BC-B73B84451793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D761FE3-8091-4547-959F-8170EF86A56D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E658BFBE-975E-47B3-8C51-826238D4C145}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="102">
   <si>
     <t>50EconomicsClassics.jpg</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Principles.jpg</t>
   </si>
   <si>
-    <t>printit.txt</t>
-  </si>
-  <si>
     <t>Reagan.jpg</t>
   </si>
   <si>
@@ -267,6 +264,81 @@
   </si>
   <si>
     <t>Thorp is cray</t>
+  </si>
+  <si>
+    <t>WhenGeniusFailed.jpg</t>
+  </si>
+  <si>
+    <t>Lying.jpg</t>
+  </si>
+  <si>
+    <t>TippingPoint.jpg</t>
+  </si>
+  <si>
+    <t>CompetitiveAdvantage.jpg</t>
+  </si>
+  <si>
+    <t>StrategicRiskTaking.jpg</t>
+  </si>
+  <si>
+    <t>PyschopathWhisperer.jpg</t>
+  </si>
+  <si>
+    <t>MalcomX.jpg</t>
+  </si>
+  <si>
+    <t>PortableFinancialAnalyst.jpg</t>
+  </si>
+  <si>
+    <t>FlashBoys.jpg</t>
+  </si>
+  <si>
+    <t>Boomerang.jpg</t>
+  </si>
+  <si>
+    <t>BigShort.jpg</t>
+  </si>
+  <si>
+    <t>BlindWatchmaker.jpg</t>
+  </si>
+  <si>
+    <t>Liar'sPoker.jpg</t>
+  </si>
+  <si>
+    <t>WinningTheLoser'sGame.jpg</t>
+  </si>
+  <si>
+    <t>MoneyChangesEverything.jpg</t>
+  </si>
+  <si>
+    <t>Seveneves.jpg</t>
+  </si>
+  <si>
+    <t>DeathByBlackHole.jpg</t>
+  </si>
+  <si>
+    <t>StuffMatters.jpg</t>
+  </si>
+  <si>
+    <t>ForTheLoveOfPhysics.jpg</t>
+  </si>
+  <si>
+    <t>InvestingPsychology.jpg</t>
+  </si>
+  <si>
+    <t>NarrativeAndNumbers.jpg</t>
+  </si>
+  <si>
+    <t>PioneeringPortfolioManagement.jpg</t>
+  </si>
+  <si>
+    <t>ASOIAF.jpg</t>
+  </si>
+  <si>
+    <t>GunsGermsSteel.jpg</t>
+  </si>
+  <si>
+    <t>HouseOfMorgan.jpg</t>
   </si>
 </sst>
 </file>
@@ -618,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CB5E06-FA96-4FE9-8E4F-D25936EA3EDB}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,16 +707,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -652,16 +724,16 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -669,16 +741,16 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -686,16 +758,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -703,16 +775,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -720,16 +792,16 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -737,16 +809,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -754,16 +826,16 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -771,16 +843,16 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -788,16 +860,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -805,16 +877,16 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -822,16 +894,16 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -839,16 +911,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -856,16 +928,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -873,16 +945,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -890,16 +962,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -907,16 +979,16 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -924,16 +996,16 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -941,16 +1013,16 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -958,16 +1030,16 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -975,16 +1047,16 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -992,16 +1064,16 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1009,16 +1081,16 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1026,16 +1098,16 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1043,16 +1115,16 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1060,16 +1132,16 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1077,16 +1149,16 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1094,16 +1166,16 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1111,16 +1183,16 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1128,16 +1200,16 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1145,16 +1217,16 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1162,16 +1234,16 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1179,16 +1251,16 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1196,16 +1268,16 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1213,16 +1285,16 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1230,16 +1302,16 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1247,16 +1319,16 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1264,16 +1336,16 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" t="s">
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1281,16 +1353,16 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C39" t="s">
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1298,16 +1370,16 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1315,16 +1387,16 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
         <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1332,16 +1404,16 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" t="s">
         <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1349,16 +1421,16 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
         <v>41</v>
       </c>
       <c r="D43" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1366,16 +1438,16 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
         <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1383,16 +1455,16 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
         <v>43</v>
       </c>
       <c r="D45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1400,16 +1472,16 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
         <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1417,16 +1489,16 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C47" t="s">
         <v>45</v>
       </c>
       <c r="D47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1434,16 +1506,16 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
         <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1451,16 +1523,16 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" t="s">
         <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1468,16 +1540,16 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" t="s">
         <v>48</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,16 +1557,16 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" t="s">
         <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1502,16 +1574,16 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" t="s">
         <v>50</v>
       </c>
       <c r="D52" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="E52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1519,16 +1591,16 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
         <v>51</v>
       </c>
       <c r="D53" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="E53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1536,16 +1608,16 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" t="s">
         <v>52</v>
       </c>
       <c r="D54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1553,16 +1625,16 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55" t="s">
         <v>53</v>
       </c>
       <c r="D55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1570,16 +1642,16 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" t="s">
         <v>54</v>
       </c>
       <c r="D56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1587,16 +1659,16 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C57" t="s">
         <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1604,16 +1676,16 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58" t="s">
         <v>56</v>
       </c>
       <c r="D58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1621,16 +1693,16 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59" t="s">
         <v>57</v>
       </c>
       <c r="D59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1638,16 +1710,16 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
         <v>58</v>
       </c>
       <c r="D60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1655,16 +1727,16 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C61" t="s">
         <v>59</v>
       </c>
       <c r="D61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1672,16 +1744,16 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62" t="s">
         <v>60</v>
       </c>
       <c r="D62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1689,16 +1761,16 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D63" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1706,16 +1778,16 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1723,16 +1795,424 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E65" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" t="s">
+        <v>62</v>
+      </c>
+      <c r="E67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" t="s">
+        <v>80</v>
+      </c>
+      <c r="D68" t="s">
+        <v>62</v>
+      </c>
+      <c r="E68" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" t="s">
+        <v>81</v>
+      </c>
+      <c r="D69" t="s">
+        <v>62</v>
+      </c>
+      <c r="E69" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C70" t="s">
+        <v>82</v>
+      </c>
+      <c r="D70" t="s">
+        <v>62</v>
+      </c>
+      <c r="E70" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>63</v>
+      </c>
+      <c r="C71" t="s">
+        <v>83</v>
+      </c>
+      <c r="D71" t="s">
+        <v>62</v>
+      </c>
+      <c r="E71" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" t="s">
+        <v>84</v>
+      </c>
+      <c r="D72" t="s">
+        <v>62</v>
+      </c>
+      <c r="E72" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" t="s">
+        <v>85</v>
+      </c>
+      <c r="D73" t="s">
+        <v>62</v>
+      </c>
+      <c r="E73" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>63</v>
+      </c>
+      <c r="C74" t="s">
+        <v>86</v>
+      </c>
+      <c r="D74" t="s">
+        <v>62</v>
+      </c>
+      <c r="E74" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>63</v>
+      </c>
+      <c r="C75" t="s">
+        <v>87</v>
+      </c>
+      <c r="D75" t="s">
+        <v>62</v>
+      </c>
+      <c r="E75" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>63</v>
+      </c>
+      <c r="C76" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76" t="s">
+        <v>62</v>
+      </c>
+      <c r="E76" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" t="s">
+        <v>89</v>
+      </c>
+      <c r="D77" t="s">
+        <v>62</v>
+      </c>
+      <c r="E77" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" t="s">
+        <v>90</v>
+      </c>
+      <c r="D78" t="s">
+        <v>62</v>
+      </c>
+      <c r="E78" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>63</v>
+      </c>
+      <c r="C79" t="s">
+        <v>91</v>
+      </c>
+      <c r="D79" t="s">
+        <v>62</v>
+      </c>
+      <c r="E79" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>63</v>
+      </c>
+      <c r="C80" t="s">
+        <v>92</v>
+      </c>
+      <c r="D80" t="s">
+        <v>62</v>
+      </c>
+      <c r="E80" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>63</v>
+      </c>
+      <c r="C81" t="s">
+        <v>93</v>
+      </c>
+      <c r="D81" t="s">
+        <v>62</v>
+      </c>
+      <c r="E81" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>63</v>
+      </c>
+      <c r="C82" t="s">
+        <v>94</v>
+      </c>
+      <c r="D82" t="s">
+        <v>62</v>
+      </c>
+      <c r="E82" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>63</v>
+      </c>
+      <c r="C83" t="s">
+        <v>95</v>
+      </c>
+      <c r="D83" t="s">
+        <v>62</v>
+      </c>
+      <c r="E83" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>63</v>
+      </c>
+      <c r="C84" t="s">
+        <v>96</v>
+      </c>
+      <c r="D84" t="s">
+        <v>62</v>
+      </c>
+      <c r="E84" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>63</v>
+      </c>
+      <c r="C85" t="s">
+        <v>97</v>
+      </c>
+      <c r="D85" t="s">
+        <v>62</v>
+      </c>
+      <c r="E85" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>63</v>
+      </c>
+      <c r="C86" t="s">
+        <v>98</v>
+      </c>
+      <c r="D86" t="s">
+        <v>62</v>
+      </c>
+      <c r="E86" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>63</v>
+      </c>
+      <c r="C87" t="s">
+        <v>99</v>
+      </c>
+      <c r="D87" t="s">
+        <v>62</v>
+      </c>
+      <c r="E87" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>63</v>
+      </c>
+      <c r="C88" t="s">
+        <v>100</v>
+      </c>
+      <c r="D88" t="s">
+        <v>62</v>
+      </c>
+      <c r="E88" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>63</v>
+      </c>
+      <c r="C89" t="s">
+        <v>101</v>
+      </c>
+      <c r="D89" t="s">
+        <v>62</v>
+      </c>
+      <c r="E89" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed sizing of all book images
</commit_message>
<xml_diff>
--- a/wwwroot/Data/BooksDB.xlsx
+++ b/wwwroot/Data/BooksDB.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgreen3\Desktop\FunWithBrandt\wwwroot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D761FE3-8091-4547-959F-8170EF86A56D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F90FFDD-EA74-4796-9C96-EB833D420A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E658BFBE-975E-47B3-8C51-826238D4C145}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="461">
   <si>
     <t>50EconomicsClassics.jpg</t>
   </si>
@@ -339,6 +340,1083 @@
   </si>
   <si>
     <t>HouseOfMorgan.jpg</t>
+  </si>
+  <si>
+    <t>ManWhoKnew.jpg</t>
+  </si>
+  <si>
+    <t>Outliers.jpg</t>
+  </si>
+  <si>
+    <t>Blink.jpg</t>
+  </si>
+  <si>
+    <t>ConfessionsOfAStreetAddict.jpg</t>
+  </si>
+  <si>
+    <t>ASlaveNoMore.jpg</t>
+  </si>
+  <si>
+    <t>AmericanSniper.jpg</t>
+  </si>
+  <si>
+    <t>BornToRun.jpg</t>
+  </si>
+  <si>
+    <t>WolfOfWallStreet.jpg</t>
+  </si>
+  <si>
+    <t>CompetitiveStrategy.jpg</t>
+  </si>
+  <si>
+    <t>SportsGene.jpg</t>
+  </si>
+  <si>
+    <t>DreamsFromMyFather.jpg</t>
+  </si>
+  <si>
+    <t>ThomasJeffersonAndTheTripoliPirates.jpg</t>
+  </si>
+  <si>
+    <t>OnceARunner.jpg</t>
+  </si>
+  <si>
+    <t>IrrationalExuberance.jpg</t>
+  </si>
+  <si>
+    <t>CommonStocksAndUncommonProfits.jpg</t>
+  </si>
+  <si>
+    <t>Freakonomics.jpg</t>
+  </si>
+  <si>
+    <t>Unbroken.jpg</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>Blink: The Power of Thinking Without Thinking</t>
+  </si>
+  <si>
+    <t>Gladwell, Malcolm</t>
+  </si>
+  <si>
+    <t>Outliers: The Story of Success</t>
+  </si>
+  <si>
+    <t>Idea Man</t>
+  </si>
+  <si>
+    <t>Allen, Paul</t>
+  </si>
+  <si>
+    <t>Shaky Ground: The Strange Saga of the U.S. Mortgage Giants</t>
+  </si>
+  <si>
+    <t>McLean, Bethany</t>
+  </si>
+  <si>
+    <t>Einstein: His Life and Universe</t>
+  </si>
+  <si>
+    <t>Isaacson, Walter *</t>
+  </si>
+  <si>
+    <t>The Greatest Adventures of Sherlock Homes</t>
+  </si>
+  <si>
+    <t>Doyle, Arthur Conan</t>
+  </si>
+  <si>
+    <t>A Splendid Exchange: How Trade Shaped the World from Prehistory to Today</t>
+  </si>
+  <si>
+    <t>Bernstein, William J.</t>
+  </si>
+  <si>
+    <t>The Autobiography of Benjamin Franklin</t>
+  </si>
+  <si>
+    <t>Franklin, Benjamin</t>
+  </si>
+  <si>
+    <t>The Universe in Your Hand: A Journey Through Space, Time, and Beyond</t>
+  </si>
+  <si>
+    <t>Galfard, Christophe</t>
+  </si>
+  <si>
+    <t>This Time Is Different: Eight Centuries of Financial Folly</t>
+  </si>
+  <si>
+    <t>Reinhart, Carmen M.</t>
+  </si>
+  <si>
+    <t>Chaos: Making a New Science</t>
+  </si>
+  <si>
+    <t>Gleick, James *</t>
+  </si>
+  <si>
+    <t>Cosmos</t>
+  </si>
+  <si>
+    <t>Sagan, Carl</t>
+  </si>
+  <si>
+    <t>Endymion (Hyperion Cantos, #3)</t>
+  </si>
+  <si>
+    <t>Simmons, Dan</t>
+  </si>
+  <si>
+    <t>Financial Risk Management for End Users</t>
+  </si>
+  <si>
+    <t>Chance, Don M</t>
+  </si>
+  <si>
+    <t>The Fall of Hyperion (Hyperion Cantos #2)</t>
+  </si>
+  <si>
+    <t>Hyperion (Hyperion Cantos, #1)</t>
+  </si>
+  <si>
+    <t>More Than You Know: Finding Financial Wisdom in Unconventional Places</t>
+  </si>
+  <si>
+    <t>Mauboussin, Michael J.</t>
+  </si>
+  <si>
+    <t>The Misbehavior of Markets: A Fractal View of Financial Turbulence</t>
+  </si>
+  <si>
+    <t>Mandelbrot, Benoît B.</t>
+  </si>
+  <si>
+    <t>Descartes' Error: Emotion, Reason and the Human Brain</t>
+  </si>
+  <si>
+    <t>Damasio, Antonio R.</t>
+  </si>
+  <si>
+    <t>Think Twice: Harnessing the Power of Counterintuition</t>
+  </si>
+  <si>
+    <t>Hedging Market Exposures: Identifying and Managing Market Risks</t>
+  </si>
+  <si>
+    <t>Bychuk, Oleg V.</t>
+  </si>
+  <si>
+    <t>Intuition: Knowing Beyond Logic</t>
+  </si>
+  <si>
+    <t>Osho</t>
+  </si>
+  <si>
+    <t>The Tiger: A True Story of Vengeance and Survival</t>
+  </si>
+  <si>
+    <t>Vaillant, John</t>
+  </si>
+  <si>
+    <t>Antifragile: Things That Gain from Disorder</t>
+  </si>
+  <si>
+    <t>Taleb, Nassim Nicholas *</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Deathly Hallows (Harry Potter, #7)</t>
+  </si>
+  <si>
+    <t>Rowling, J.K.</t>
+  </si>
+  <si>
+    <t>Harry Potter Collection (Harry Potter, #1-6)</t>
+  </si>
+  <si>
+    <t>Steve Jobs</t>
+  </si>
+  <si>
+    <t>Born a Crime: Stories from a South African Childhood</t>
+  </si>
+  <si>
+    <t>Noah, Trevor</t>
+  </si>
+  <si>
+    <t>"Surely You're Joking, Mr. Feynman!": Adventures of a Curious Character</t>
+  </si>
+  <si>
+    <t>Feynman, Richard</t>
+  </si>
+  <si>
+    <t>Principles: Life and Work</t>
+  </si>
+  <si>
+    <t>Dalio, Ray *</t>
+  </si>
+  <si>
+    <t>All the Devils are Here: The Hidden History of the Financial Crisis</t>
+  </si>
+  <si>
+    <t>The Checklist Manifesto: How to Get Things Right</t>
+  </si>
+  <si>
+    <t>Gawande, Atul</t>
+  </si>
+  <si>
+    <t>The Worldly Philosophers</t>
+  </si>
+  <si>
+    <t>Heilbroner, Robert L.</t>
+  </si>
+  <si>
+    <t>Strategic Value Investing: Techniques from the World's Leadistrategic Value Investing: Techniques from the World's Leading Value Investors of All Time Ng Value Investors of All Time</t>
+  </si>
+  <si>
+    <t>Horan, Stephen M.</t>
+  </si>
+  <si>
+    <t>Naked Money: A Revealing Look at What It Is and Why It Matters</t>
+  </si>
+  <si>
+    <t>Wheelan, Charles</t>
+  </si>
+  <si>
+    <t>Enlightenment Now: The Case for Reason, Science, Humanism, and Progress</t>
+  </si>
+  <si>
+    <t>Pinker, Steven *</t>
+  </si>
+  <si>
+    <t>Crashed: How a Decade of Financial Crises Changed the World</t>
+  </si>
+  <si>
+    <t>Tooze, Adam</t>
+  </si>
+  <si>
+    <t>Oil 101</t>
+  </si>
+  <si>
+    <t>Downey, Morgan Patrick</t>
+  </si>
+  <si>
+    <t>Understanding Hedge Fund Investing + Web-Based Software: How to Invest in Alternative Assets and Manage Risk/Return</t>
+  </si>
+  <si>
+    <t>Mirabile, Kevin R.</t>
+  </si>
+  <si>
+    <t>A Man for All Markets</t>
+  </si>
+  <si>
+    <t>Thorp, Edward O.</t>
+  </si>
+  <si>
+    <t>Napoleon: A Life</t>
+  </si>
+  <si>
+    <t>Roberts, Andrew</t>
+  </si>
+  <si>
+    <t>50 Economics Classics: Your shortcut to the most important ideas on capitalism, finance, and the global economy</t>
+  </si>
+  <si>
+    <t>Butler-Bowdon, Tom *</t>
+  </si>
+  <si>
+    <t>Capital in the Twenty-First Century</t>
+  </si>
+  <si>
+    <t>Piketty, Thomas</t>
+  </si>
+  <si>
+    <t>Adam Smith: Father of Economics</t>
+  </si>
+  <si>
+    <t>Norman, Jesse</t>
+  </si>
+  <si>
+    <t>Capital Ideas Evolving</t>
+  </si>
+  <si>
+    <t>Bernstein, Peter L.</t>
+  </si>
+  <si>
+    <t>Mastering the Market Cycle: Getting the Odds on Your Side</t>
+  </si>
+  <si>
+    <t>Marks, Howard</t>
+  </si>
+  <si>
+    <t>The Four: The Hidden DNA of Amazon, Apple, Facebook, and Google</t>
+  </si>
+  <si>
+    <t>Galloway, Scott</t>
+  </si>
+  <si>
+    <t>The Snowball: Warren Buffett and the Business of Life</t>
+  </si>
+  <si>
+    <t>Schroeder, Alice</t>
+  </si>
+  <si>
+    <t>Reagan: The Life</t>
+  </si>
+  <si>
+    <t>Brands, H.W.</t>
+  </si>
+  <si>
+    <t>Moonwalking with Einstein: The Art and Science of Remembering Everything</t>
+  </si>
+  <si>
+    <t>Foer, Joshua *</t>
+  </si>
+  <si>
+    <t>Naked Economics: Undressing the Dismal Science</t>
+  </si>
+  <si>
+    <t>Algebra II for Dummies</t>
+  </si>
+  <si>
+    <t>Sterling</t>
+  </si>
+  <si>
+    <t>Statistics for Dummies, 2nd Edition</t>
+  </si>
+  <si>
+    <t>Rumsey, Deborah J.</t>
+  </si>
+  <si>
+    <t>Too Big to Fail: The Inside Story of How Wall Street and Washington Fought to Save the Financial System from Crisis — and Themselves</t>
+  </si>
+  <si>
+    <t>Sorkin, Andrew Ross</t>
+  </si>
+  <si>
+    <t>In an Uncertain World: Tough Choices from Wall Street to Washington</t>
+  </si>
+  <si>
+    <t>Rubin, Robert E.</t>
+  </si>
+  <si>
+    <t>The Age of Turbulence: Adventures in a New World</t>
+  </si>
+  <si>
+    <t>Greenspan, Alan</t>
+  </si>
+  <si>
+    <t>Dealing with China: An Insider Unmasks the New Economic Superpower</t>
+  </si>
+  <si>
+    <t>Paulson, Henry M. Jr.</t>
+  </si>
+  <si>
+    <t>Behave: The Biology of Humans at Our Best and Worst</t>
+  </si>
+  <si>
+    <t>Sapolsky, Robert M.</t>
+  </si>
+  <si>
+    <t>A Demon of Our Own Design: Markets, Hedge Funds, and the Perils of Financial Innovation</t>
+  </si>
+  <si>
+    <t>Bookstaber, Richard</t>
+  </si>
+  <si>
+    <t>Predicting the Markets: A Professional Autobiography</t>
+  </si>
+  <si>
+    <t>Yardeni, Edward</t>
+  </si>
+  <si>
+    <t>Against the Gods: The Remarkable Story of Risk</t>
+  </si>
+  <si>
+    <t>The Black Swan: The Impact of the Highly Improbable</t>
+  </si>
+  <si>
+    <t>Lords of Finance: The Bankers Who Broke the World</t>
+  </si>
+  <si>
+    <t>Ahamed, Liaquat</t>
+  </si>
+  <si>
+    <t>Superfreakonomics: A Rogue Economist Explores the Hidden Side of Everything</t>
+  </si>
+  <si>
+    <t>Levitt, Steven D.</t>
+  </si>
+  <si>
+    <t>The Magic of Reality: How We Know What's Really True</t>
+  </si>
+  <si>
+    <t>Dawkins, Richard *</t>
+  </si>
+  <si>
+    <t>Leonardo da Vinci</t>
+  </si>
+  <si>
+    <t>Elon Musk: Tesla, SpaceX, and the Quest for a Fantastic Future</t>
+  </si>
+  <si>
+    <t>Vance, Ashlee *</t>
+  </si>
+  <si>
+    <t>Subliminal: How Your Unconscious Mind Rules Your Behavior</t>
+  </si>
+  <si>
+    <t>Mlodinow, Leonard</t>
+  </si>
+  <si>
+    <t>A Random Walk Down Wall Street</t>
+  </si>
+  <si>
+    <t>Malkiel, Burton G.</t>
+  </si>
+  <si>
+    <t>The Hero With a Thousand Faces</t>
+  </si>
+  <si>
+    <t>Campbell, Joseph</t>
+  </si>
+  <si>
+    <t>Benjamin Franklin: An American Life</t>
+  </si>
+  <si>
+    <t>The Undoing Project: A Friendship That Changed Our Minds</t>
+  </si>
+  <si>
+    <t>Lewis, Michael</t>
+  </si>
+  <si>
+    <t>The Gene: An Intimate History</t>
+  </si>
+  <si>
+    <t>Mukherjee, Siddhartha</t>
+  </si>
+  <si>
+    <t>When Genius Failed: The Rise and Fall of Long-Term Capital Management</t>
+  </si>
+  <si>
+    <t>Lowenstein, Roger</t>
+  </si>
+  <si>
+    <t>Lying</t>
+  </si>
+  <si>
+    <t>Harris, Sam</t>
+  </si>
+  <si>
+    <t>The Tipping Point: How Little Things Can Make a Big Difference</t>
+  </si>
+  <si>
+    <t>Competitive Advantage: Creating and Sustaining Superior Performance</t>
+  </si>
+  <si>
+    <t>Porter, Michael E.</t>
+  </si>
+  <si>
+    <t>Strategic Risk Taking: A Framework For Risk Management</t>
+  </si>
+  <si>
+    <t>Damodaran, Aswath</t>
+  </si>
+  <si>
+    <t>The Psychopath Whisperer: The Science of Those Without Conscience</t>
+  </si>
+  <si>
+    <t>Kiehl, Kent</t>
+  </si>
+  <si>
+    <t>The Autobiography of Malcolm X</t>
+  </si>
+  <si>
+    <t>X, Malcolm</t>
+  </si>
+  <si>
+    <t>The Portable Financial Analyst: What Practitioners Need to Know</t>
+  </si>
+  <si>
+    <t>Kritzman, Mark P.</t>
+  </si>
+  <si>
+    <t>Flash Boys: A Wall Street Revolt</t>
+  </si>
+  <si>
+    <t>Boomerang: Travels in the New Third World</t>
+  </si>
+  <si>
+    <t>The Big Short: Inside the Doomsday Machine</t>
+  </si>
+  <si>
+    <t>The Blind Watchmaker: Why the Evidence of Evolution Reveals a Universe Without Design</t>
+  </si>
+  <si>
+    <t>Fooled by Randomness: The Hidden Role of Chance in Life and in the Markets</t>
+  </si>
+  <si>
+    <t>Liar's Poker</t>
+  </si>
+  <si>
+    <t>Winning the Loser's Game: Timeless Strategies for Successful Investing</t>
+  </si>
+  <si>
+    <t>Ellis, Charles D.</t>
+  </si>
+  <si>
+    <t>Money Changes Everything: How Finance Made Civilization Possible</t>
+  </si>
+  <si>
+    <t>Goetzmann, William N.</t>
+  </si>
+  <si>
+    <t>Seveneves</t>
+  </si>
+  <si>
+    <t>Stephenson, Neal *</t>
+  </si>
+  <si>
+    <t>Death by Black Hole: And Other Cosmic Quandaries</t>
+  </si>
+  <si>
+    <t>Tyson, Neil deGrasse *</t>
+  </si>
+  <si>
+    <t>Stuff Matters: Exploring the Marvelous Materials That Shape Our Man-Made World</t>
+  </si>
+  <si>
+    <t>Miodownik, Mark</t>
+  </si>
+  <si>
+    <t>For the Love of Physics: From the End of the Rainbow to the Edge of Time - A Journey Through the Wonders of Physics</t>
+  </si>
+  <si>
+    <t>Lewin, Walter</t>
+  </si>
+  <si>
+    <t>Hard Contact (Star Wars: Republic Commando, #1)</t>
+  </si>
+  <si>
+    <t>Traviss, Karen *</t>
+  </si>
+  <si>
+    <t>Investing Psychology + Ws</t>
+  </si>
+  <si>
+    <t>Richards, Tim</t>
+  </si>
+  <si>
+    <t>Narrative and Numbers: The Value of Stories in Business</t>
+  </si>
+  <si>
+    <t>Focus Groups: Hitting the Bull's-Eye</t>
+  </si>
+  <si>
+    <t>Miller, Phillip H.</t>
+  </si>
+  <si>
+    <t>Pioneering Portfolio Management: An Unconventional Approach to Institutional Investment, Fully Revised and Updated</t>
+  </si>
+  <si>
+    <t>Swensen, David F.</t>
+  </si>
+  <si>
+    <t>A Game of Thrones (A Song of Ice and Fire, #1)</t>
+  </si>
+  <si>
+    <t>Martin, George R.R.</t>
+  </si>
+  <si>
+    <t>Art of Lawyering</t>
+  </si>
+  <si>
+    <t>Lisnek, Paul M.</t>
+  </si>
+  <si>
+    <t>Guns, Germs, and Steel: The Fates of Human Societies</t>
+  </si>
+  <si>
+    <t>Diamond, Jared</t>
+  </si>
+  <si>
+    <t>The House of Morgan: An American Banking Dynasty and the Rise of Modern Finance</t>
+  </si>
+  <si>
+    <t>Chernow, Ron</t>
+  </si>
+  <si>
+    <t>The Man Who Knew: The Life and Times of Alan Greenspan</t>
+  </si>
+  <si>
+    <t>Mallaby, Sebastian</t>
+  </si>
+  <si>
+    <t>Wicked: The Life and Times of the Wicked Witch of the West (The Wicked Years, #1)</t>
+  </si>
+  <si>
+    <t>Maguire, Gregory</t>
+  </si>
+  <si>
+    <t>The Sister of the South (Dragons of Deltora, #4)</t>
+  </si>
+  <si>
+    <t>Rodda, Emily *</t>
+  </si>
+  <si>
+    <t>Isle of the Dead (Dragons of Deltora, #3)</t>
+  </si>
+  <si>
+    <t>Shadowgate (Dragons of Deltora, #2)</t>
+  </si>
+  <si>
+    <t>Dragon's Nest (Dragons of Deltora, #1)</t>
+  </si>
+  <si>
+    <t>Falling Kingdoms (Falling Kingdoms, #1)</t>
+  </si>
+  <si>
+    <t>Rhodes, Morgan *</t>
+  </si>
+  <si>
+    <t>The Death Cure (The Maze Runner, #3)</t>
+  </si>
+  <si>
+    <t>Dashner, James *</t>
+  </si>
+  <si>
+    <t>The Scorch Trials (The Maze Runner, #2)</t>
+  </si>
+  <si>
+    <t>The Maze Runner (The Maze Runner, #1)</t>
+  </si>
+  <si>
+    <t>The Enchanter Heir (The Heir Chronicles, #4)</t>
+  </si>
+  <si>
+    <t>Chima, Cinda Williams *</t>
+  </si>
+  <si>
+    <t>The Dragon Heir (The Heir Chronicles, #3)</t>
+  </si>
+  <si>
+    <t>The Crimson Crown (Seven Realms, #4)</t>
+  </si>
+  <si>
+    <t>The Gray Wolf Throne (Seven Realms, #3)</t>
+  </si>
+  <si>
+    <t>The Wizard Heir (The Heir Chronicles, #2)</t>
+  </si>
+  <si>
+    <t>The Exiled Queen (Seven Realms, #2)</t>
+  </si>
+  <si>
+    <t>The Demon King (Seven Realms, #1)</t>
+  </si>
+  <si>
+    <t>The Warrior Heir (The Heir Chronicles, #1)</t>
+  </si>
+  <si>
+    <t>The Inkheart Trilogy: Inkheart, Inkspell, Inkdeath</t>
+  </si>
+  <si>
+    <t>Funke, Cornelia *</t>
+  </si>
+  <si>
+    <t>The Blood of Olympus (The Heroes of Olympus, #5)</t>
+  </si>
+  <si>
+    <t>Riordan, Rick *</t>
+  </si>
+  <si>
+    <t>The House of Hades (The Heroes of Olympus, #4)</t>
+  </si>
+  <si>
+    <t>The Mark of Athena (The Heroes of Olympus, #3)</t>
+  </si>
+  <si>
+    <t>The Son of Neptune (The Heroes of Olympus, #2)</t>
+  </si>
+  <si>
+    <t>The Lost Hero (The Heroes of Olympus, #1)</t>
+  </si>
+  <si>
+    <t>The Titan's Curse (Percy Jackson and the Olympians, #3)</t>
+  </si>
+  <si>
+    <t>The Last Olympian (Percy Jackson and the Olympians, #5)</t>
+  </si>
+  <si>
+    <t>The Sea of Monsters (Percy Jackson and the Olympians, #2)</t>
+  </si>
+  <si>
+    <t>The Battle of the Labyrinth (Percy Jackson and the Olympians, #4)</t>
+  </si>
+  <si>
+    <t>The Lightning Thief (Percy Jackson and the Olympians, #1)</t>
+  </si>
+  <si>
+    <t>Inheritance (The Inheritance Cycle, #4)</t>
+  </si>
+  <si>
+    <t>Paolini, Christopher *</t>
+  </si>
+  <si>
+    <t>Brisingr (The Inheritance Cycle, #3)</t>
+  </si>
+  <si>
+    <t>Eldest (The Inheritance Cycle, #2)</t>
+  </si>
+  <si>
+    <t>Eragon (The Inheritance Cycle, #1)</t>
+  </si>
+  <si>
+    <t>The Lost Stories (Ranger's Apprentice, #11)</t>
+  </si>
+  <si>
+    <t>Flanagan, John</t>
+  </si>
+  <si>
+    <t>The Emperor of Nihon-Ja (Ranger's Apprentice, #10)</t>
+  </si>
+  <si>
+    <t>Halt's Peril (Ranger's Apprentice, #9)</t>
+  </si>
+  <si>
+    <t>The Kings of Clonmel (Ranger's Apprentice, #8)</t>
+  </si>
+  <si>
+    <t>Erak's Ransom (Ranger's Apprentice, #7)</t>
+  </si>
+  <si>
+    <t>The Siege of Macindaw (Ranger's Apprentice, #6)</t>
+  </si>
+  <si>
+    <t>The Sorcerer of the North (Ranger's Apprentice, #5)</t>
+  </si>
+  <si>
+    <t>The Icebound Land (Ranger's Apprentice, #3)</t>
+  </si>
+  <si>
+    <t>The Battle for Skandia (Ranger's Apprentice, #4)</t>
+  </si>
+  <si>
+    <t>The Royal Ranger (Ranger's Apprentice #12 Ranger's Apprentice: The Royal Ranger #1)</t>
+  </si>
+  <si>
+    <t>The Burning Bridge (Ranger's Apprentice, #2)</t>
+  </si>
+  <si>
+    <t>The Ruins of Gorlan (Ranger's Apprentice, #1)</t>
+  </si>
+  <si>
+    <t>Scorpia Rising (Alex Rider, #9)</t>
+  </si>
+  <si>
+    <t>Horowitz, Anthony *</t>
+  </si>
+  <si>
+    <t>Crocodile Tears (Alex Rider, #8)</t>
+  </si>
+  <si>
+    <t>Snakehead (Alex Rider, #7)</t>
+  </si>
+  <si>
+    <t>Ark Angel (Alex Rider, #6)</t>
+  </si>
+  <si>
+    <t>Scorpia (Alex Rider, #5)</t>
+  </si>
+  <si>
+    <t>Eagle Strike (Alex Rider, #4)</t>
+  </si>
+  <si>
+    <t>Skeleton Key (Alex Rider, #3)</t>
+  </si>
+  <si>
+    <t>Point Blank (Alex Rider, #2)</t>
+  </si>
+  <si>
+    <t>Stormbreaker (Alex Rider, #1)</t>
+  </si>
+  <si>
+    <t>Ptolemy's Gate (Bartimaeus, #3)</t>
+  </si>
+  <si>
+    <t>Stroud, Jonathan *</t>
+  </si>
+  <si>
+    <t>The Golem's Eye (Bartimaeus, #2)</t>
+  </si>
+  <si>
+    <t>The Amulet of Samarkand (Bartimaeus, #1)</t>
+  </si>
+  <si>
+    <t>The Brethren</t>
+  </si>
+  <si>
+    <t>Grisham, John *</t>
+  </si>
+  <si>
+    <t>Inferno (Robert Langdon, #4)</t>
+  </si>
+  <si>
+    <t>Brown, Dan *</t>
+  </si>
+  <si>
+    <t>The Lost Symbol (Robert Langdon, #3)</t>
+  </si>
+  <si>
+    <t>Night (The Night Trilogy, #1)</t>
+  </si>
+  <si>
+    <t>Wiesel, Elie</t>
+  </si>
+  <si>
+    <t>Of Mice and Men</t>
+  </si>
+  <si>
+    <t>Steinbeck, John</t>
+  </si>
+  <si>
+    <t>Inherit the Wind</t>
+  </si>
+  <si>
+    <t>Lawrence, Jerome</t>
+  </si>
+  <si>
+    <t>Confessions of a Street Addict</t>
+  </si>
+  <si>
+    <t>Cramer, James J.</t>
+  </si>
+  <si>
+    <t>A Knight of the Seven Kingdoms (The Tales of Dunk and Egg, #1-3)</t>
+  </si>
+  <si>
+    <t>The Book Thief</t>
+  </si>
+  <si>
+    <t>Zusak, Markus *</t>
+  </si>
+  <si>
+    <t>The Curious Incident of the Dog in the Night-Time</t>
+  </si>
+  <si>
+    <t>Haddon, Mark</t>
+  </si>
+  <si>
+    <t>A Streetcar Named Desire</t>
+  </si>
+  <si>
+    <t>Williams, Tennessee</t>
+  </si>
+  <si>
+    <t>The Old Man and the Sea</t>
+  </si>
+  <si>
+    <t>Hemingway, Ernest</t>
+  </si>
+  <si>
+    <t>Zen and the Art of Motorcycle Maintenance: An Inquiry Into Values (Phaedrus, #1)</t>
+  </si>
+  <si>
+    <t>Pirsig, Robert M.</t>
+  </si>
+  <si>
+    <t>Into the Wild</t>
+  </si>
+  <si>
+    <t>Krakauer, Jon *</t>
+  </si>
+  <si>
+    <t>A Clash of Kings (A Song of Ice and Fire, #2)</t>
+  </si>
+  <si>
+    <t>A Feast for Crows (A Song of Ice and Fire, #4)</t>
+  </si>
+  <si>
+    <t>A Storm of Swords (A Song of Ice and Fire, #3)</t>
+  </si>
+  <si>
+    <t>A Dance with Dragons (A Song of Ice and Fire, #5)</t>
+  </si>
+  <si>
+    <t>Brave New World</t>
+  </si>
+  <si>
+    <t>Huxley, Aldous</t>
+  </si>
+  <si>
+    <t>Divergent (Divergent, #1)</t>
+  </si>
+  <si>
+    <t>Roth, Veronica *</t>
+  </si>
+  <si>
+    <t>To Kill a Mockingbird</t>
+  </si>
+  <si>
+    <t>Lee, Harper</t>
+  </si>
+  <si>
+    <t>Mockingjay (The Hunger Games, #3)</t>
+  </si>
+  <si>
+    <t>Collins, Suzanne</t>
+  </si>
+  <si>
+    <t>Catching Fire (The Hunger Games, #2)</t>
+  </si>
+  <si>
+    <t>A Slave No More: Two Men Who Escaped to Freedom, Including Their Own Narratives of Emancipation</t>
+  </si>
+  <si>
+    <t>Blight, David W.</t>
+  </si>
+  <si>
+    <t>American Sniper: The Autobiography of the Most Lethal Sniper in U.S. Military History</t>
+  </si>
+  <si>
+    <t>Kyle, Chris</t>
+  </si>
+  <si>
+    <t>The Dynamics of Persuasion: Communication and Attitudes in the 21st Century</t>
+  </si>
+  <si>
+    <t>Perloff, Richard M.</t>
+  </si>
+  <si>
+    <t>The National Debt of the United States, 1941 to 2008</t>
+  </si>
+  <si>
+    <t>Kelly, Robert E.</t>
+  </si>
+  <si>
+    <t>Dune (Dune Chronicles, #1)</t>
+  </si>
+  <si>
+    <t>Herbert, Frank</t>
+  </si>
+  <si>
+    <t>Dune Messiah (Dune Chronicles #2)</t>
+  </si>
+  <si>
+    <t>Born to Run: A Hidden Tribe, Superathletes, and the Greatest Race the World Has Never Seen</t>
+  </si>
+  <si>
+    <t>McDougall, Christopher</t>
+  </si>
+  <si>
+    <t>The Wolf of Wall Street (The Wolf of Wall Street, #1)</t>
+  </si>
+  <si>
+    <t>Belfort, Jordan *</t>
+  </si>
+  <si>
+    <t>The Heart and the Fist: The Education of a Humanitarian, the Making of a Navy SEAL</t>
+  </si>
+  <si>
+    <t>Greitens, Eric</t>
+  </si>
+  <si>
+    <t>Competitive Strategy: Techniques for Analyzing Industries and Competitors</t>
+  </si>
+  <si>
+    <t>Orwell, George</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings (The Lord of the Rings, #1-3)</t>
+  </si>
+  <si>
+    <t>Tolkien, J.R.R.</t>
+  </si>
+  <si>
+    <t>The Sports Gene: Inside the Science of Extraordinary Athletic Performance</t>
+  </si>
+  <si>
+    <t>Epstein, David *</t>
+  </si>
+  <si>
+    <t>The Da Vinci Code (Robert Langdon, #2)</t>
+  </si>
+  <si>
+    <t>Dreams from My Father: A Story of Race and Inheritance</t>
+  </si>
+  <si>
+    <t>Obama, Barack</t>
+  </si>
+  <si>
+    <t>Stress Test: Reflections on Financial Crises</t>
+  </si>
+  <si>
+    <t>Geithner, Timothy F.</t>
+  </si>
+  <si>
+    <t>The Courage to Act: A Memoir of a Crisis and Its Aftermath</t>
+  </si>
+  <si>
+    <t>Bernanke, Ben S.</t>
+  </si>
+  <si>
+    <t>Thomas Jefferson and the Tripoli Pirates: The Forgotten War that Changed American History</t>
+  </si>
+  <si>
+    <t>Kilmeade, Brian</t>
+  </si>
+  <si>
+    <t>Once a Runner</t>
+  </si>
+  <si>
+    <t>Parker Jr., John L.</t>
+  </si>
+  <si>
+    <t>The Once and Future King (The Once and Future King, #1-4)</t>
+  </si>
+  <si>
+    <t>White, T.H.</t>
+  </si>
+  <si>
+    <t>Irrational Exuberance</t>
+  </si>
+  <si>
+    <t>Shiller, Robert J.</t>
+  </si>
+  <si>
+    <t>The Hobbit</t>
+  </si>
+  <si>
+    <t>The Hunger Games (The Hunger Games, #1)</t>
+  </si>
+  <si>
+    <t>Fahrenheit 451</t>
+  </si>
+  <si>
+    <t>Bradbury, Ray</t>
+  </si>
+  <si>
+    <t>Common Stocks and Uncommon Profits and Other Writings</t>
+  </si>
+  <si>
+    <t>Fisher, Philip A.</t>
+  </si>
+  <si>
+    <t>Freakonomics: A Rogue Economist Explores the Hidden Side of Everything</t>
+  </si>
+  <si>
+    <t>Unbroken: A World War II Story of Survival, Resilience and Redemption</t>
+  </si>
+  <si>
+    <t>Hillenbrand, Laura</t>
+  </si>
+  <si>
+    <t>date added Down arrow</t>
   </si>
 </sst>
 </file>
@@ -374,8 +1452,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,16 +1769,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CB5E06-FA96-4FE9-8E4F-D25936EA3EDB}">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2215,6 +3293,2624 @@
         <v>64</v>
       </c>
     </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>63</v>
+      </c>
+      <c r="C90" t="s">
+        <v>102</v>
+      </c>
+      <c r="D90" t="s">
+        <v>62</v>
+      </c>
+      <c r="E90" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>63</v>
+      </c>
+      <c r="C91" t="s">
+        <v>103</v>
+      </c>
+      <c r="D91" t="s">
+        <v>62</v>
+      </c>
+      <c r="E91" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>63</v>
+      </c>
+      <c r="C92" t="s">
+        <v>104</v>
+      </c>
+      <c r="D92" t="s">
+        <v>62</v>
+      </c>
+      <c r="E92" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
+        <v>63</v>
+      </c>
+      <c r="C93" t="s">
+        <v>105</v>
+      </c>
+      <c r="D93" t="s">
+        <v>62</v>
+      </c>
+      <c r="E93" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
+        <v>63</v>
+      </c>
+      <c r="C94" t="s">
+        <v>106</v>
+      </c>
+      <c r="D94" t="s">
+        <v>62</v>
+      </c>
+      <c r="E94" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>63</v>
+      </c>
+      <c r="C95" t="s">
+        <v>107</v>
+      </c>
+      <c r="D95" t="s">
+        <v>62</v>
+      </c>
+      <c r="E95" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>63</v>
+      </c>
+      <c r="C96" t="s">
+        <v>108</v>
+      </c>
+      <c r="D96" t="s">
+        <v>62</v>
+      </c>
+      <c r="E96" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>97</v>
+      </c>
+      <c r="B97" t="s">
+        <v>63</v>
+      </c>
+      <c r="C97" t="s">
+        <v>109</v>
+      </c>
+      <c r="D97" t="s">
+        <v>62</v>
+      </c>
+      <c r="E97" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>98</v>
+      </c>
+      <c r="B98" t="s">
+        <v>63</v>
+      </c>
+      <c r="C98" t="s">
+        <v>110</v>
+      </c>
+      <c r="D98" t="s">
+        <v>62</v>
+      </c>
+      <c r="E98" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>99</v>
+      </c>
+      <c r="B99" t="s">
+        <v>63</v>
+      </c>
+      <c r="C99" t="s">
+        <v>111</v>
+      </c>
+      <c r="D99" t="s">
+        <v>62</v>
+      </c>
+      <c r="E99" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>100</v>
+      </c>
+      <c r="B100" t="s">
+        <v>63</v>
+      </c>
+      <c r="C100" t="s">
+        <v>112</v>
+      </c>
+      <c r="D100" t="s">
+        <v>62</v>
+      </c>
+      <c r="E100" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>101</v>
+      </c>
+      <c r="B101" t="s">
+        <v>63</v>
+      </c>
+      <c r="C101" t="s">
+        <v>113</v>
+      </c>
+      <c r="D101" t="s">
+        <v>62</v>
+      </c>
+      <c r="E101" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>102</v>
+      </c>
+      <c r="B102" t="s">
+        <v>63</v>
+      </c>
+      <c r="C102" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" t="s">
+        <v>62</v>
+      </c>
+      <c r="E102" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>103</v>
+      </c>
+      <c r="B103" t="s">
+        <v>63</v>
+      </c>
+      <c r="C103" t="s">
+        <v>115</v>
+      </c>
+      <c r="D103" t="s">
+        <v>62</v>
+      </c>
+      <c r="E103" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>104</v>
+      </c>
+      <c r="B104" t="s">
+        <v>63</v>
+      </c>
+      <c r="C104" t="s">
+        <v>116</v>
+      </c>
+      <c r="D104" t="s">
+        <v>62</v>
+      </c>
+      <c r="E104" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>105</v>
+      </c>
+      <c r="B105" t="s">
+        <v>63</v>
+      </c>
+      <c r="C105" t="s">
+        <v>117</v>
+      </c>
+      <c r="D105" t="s">
+        <v>62</v>
+      </c>
+      <c r="E105" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>63</v>
+      </c>
+      <c r="C106" t="s">
+        <v>118</v>
+      </c>
+      <c r="D106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E106" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AB8ED2-91A1-4D7D-9C24-162C8C4C0B88}">
+  <dimension ref="A1:C626"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="75.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43946</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43946</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43894</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43888</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="1">
+        <v>43869</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="1">
+        <v>43869</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="1">
+        <v>43853</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43841</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="1">
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="1">
+        <v>43826</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="1">
+        <v>43801</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" s="1">
+        <v>43781</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B44" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" s="1">
+        <v>43774</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B47" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="1">
+        <v>43755</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" s="1">
+        <v>43752</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>152</v>
+      </c>
+      <c r="B53" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" s="1">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>154</v>
+      </c>
+      <c r="B56" t="s">
+        <v>155</v>
+      </c>
+      <c r="C56" s="1">
+        <v>43701</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" s="1">
+        <v>43697</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>157</v>
+      </c>
+      <c r="B62" t="s">
+        <v>158</v>
+      </c>
+      <c r="C62" s="1">
+        <v>43692</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" s="1">
+        <v>43681</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>161</v>
+      </c>
+      <c r="B68" t="s">
+        <v>162</v>
+      </c>
+      <c r="C68" s="1">
+        <v>43667</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>163</v>
+      </c>
+      <c r="B71" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" s="1">
+        <v>43664</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>165</v>
+      </c>
+      <c r="B74" t="s">
+        <v>166</v>
+      </c>
+      <c r="C74" s="1">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>167</v>
+      </c>
+      <c r="B77" t="s">
+        <v>166</v>
+      </c>
+      <c r="C77" s="1">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>168</v>
+      </c>
+      <c r="B80" t="s">
+        <v>129</v>
+      </c>
+      <c r="C80" s="1">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>169</v>
+      </c>
+      <c r="B83" t="s">
+        <v>170</v>
+      </c>
+      <c r="C83" s="1">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" s="1">
+        <v>43606</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>173</v>
+      </c>
+      <c r="B89" t="s">
+        <v>174</v>
+      </c>
+      <c r="C89" s="1">
+        <v>43601</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>175</v>
+      </c>
+      <c r="B92" t="s">
+        <v>127</v>
+      </c>
+      <c r="C92" s="1">
+        <v>43599</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>176</v>
+      </c>
+      <c r="B95" t="s">
+        <v>177</v>
+      </c>
+      <c r="C95" s="1">
+        <v>43593</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>178</v>
+      </c>
+      <c r="B98" t="s">
+        <v>179</v>
+      </c>
+      <c r="C98" s="1">
+        <v>43573</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>180</v>
+      </c>
+      <c r="B101" t="s">
+        <v>181</v>
+      </c>
+      <c r="C101" s="1">
+        <v>43572</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>182</v>
+      </c>
+      <c r="B104" t="s">
+        <v>183</v>
+      </c>
+      <c r="C104" s="1">
+        <v>43565</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>184</v>
+      </c>
+      <c r="B107" t="s">
+        <v>185</v>
+      </c>
+      <c r="C107" s="1">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>186</v>
+      </c>
+      <c r="B110" t="s">
+        <v>187</v>
+      </c>
+      <c r="C110" s="1">
+        <v>43544</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>188</v>
+      </c>
+      <c r="B113" t="s">
+        <v>189</v>
+      </c>
+      <c r="C113" s="1">
+        <v>43541</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>190</v>
+      </c>
+      <c r="B116" t="s">
+        <v>191</v>
+      </c>
+      <c r="C116" s="1">
+        <v>43541</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>192</v>
+      </c>
+      <c r="B119" t="s">
+        <v>193</v>
+      </c>
+      <c r="C119" s="1">
+        <v>43500</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>194</v>
+      </c>
+      <c r="B122" t="s">
+        <v>195</v>
+      </c>
+      <c r="C122" s="1">
+        <v>43488</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>196</v>
+      </c>
+      <c r="B125" t="s">
+        <v>197</v>
+      </c>
+      <c r="C125" s="1">
+        <v>43460</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>198</v>
+      </c>
+      <c r="B128" t="s">
+        <v>199</v>
+      </c>
+      <c r="C128" s="1">
+        <v>43436</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>200</v>
+      </c>
+      <c r="B131" t="s">
+        <v>201</v>
+      </c>
+      <c r="C131" s="1">
+        <v>43432</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>202</v>
+      </c>
+      <c r="B134" t="s">
+        <v>203</v>
+      </c>
+      <c r="C134" s="1">
+        <v>43411</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>204</v>
+      </c>
+      <c r="B137" t="s">
+        <v>205</v>
+      </c>
+      <c r="C137" s="1">
+        <v>43411</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>206</v>
+      </c>
+      <c r="B140" t="s">
+        <v>207</v>
+      </c>
+      <c r="C140" s="1">
+        <v>43406</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>208</v>
+      </c>
+      <c r="B143" t="s">
+        <v>209</v>
+      </c>
+      <c r="C143" s="1">
+        <v>43384</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>210</v>
+      </c>
+      <c r="B146" t="s">
+        <v>211</v>
+      </c>
+      <c r="C146" s="1">
+        <v>43350</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>212</v>
+      </c>
+      <c r="B149" t="s">
+        <v>213</v>
+      </c>
+      <c r="C149" s="1">
+        <v>43329</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>214</v>
+      </c>
+      <c r="B152" t="s">
+        <v>183</v>
+      </c>
+      <c r="C152" s="1">
+        <v>43327</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>215</v>
+      </c>
+      <c r="B155" t="s">
+        <v>216</v>
+      </c>
+      <c r="C155" s="1">
+        <v>43316</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>217</v>
+      </c>
+      <c r="B158" t="s">
+        <v>218</v>
+      </c>
+      <c r="C158" s="1">
+        <v>43316</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>219</v>
+      </c>
+      <c r="B161" t="s">
+        <v>220</v>
+      </c>
+      <c r="C161" s="1">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>221</v>
+      </c>
+      <c r="B164" t="s">
+        <v>222</v>
+      </c>
+      <c r="C164" s="1">
+        <v>43303</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>223</v>
+      </c>
+      <c r="B167" t="s">
+        <v>224</v>
+      </c>
+      <c r="C167" s="1">
+        <v>43298</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>225</v>
+      </c>
+      <c r="B170" t="s">
+        <v>226</v>
+      </c>
+      <c r="C170" s="1">
+        <v>43291</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>227</v>
+      </c>
+      <c r="B173" t="s">
+        <v>228</v>
+      </c>
+      <c r="C173" s="1">
+        <v>43284</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>229</v>
+      </c>
+      <c r="B176" t="s">
+        <v>230</v>
+      </c>
+      <c r="C176" s="1">
+        <v>43260</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>231</v>
+      </c>
+      <c r="B179" t="s">
+        <v>232</v>
+      </c>
+      <c r="C179" s="1">
+        <v>43245</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>233</v>
+      </c>
+      <c r="B182" t="s">
+        <v>203</v>
+      </c>
+      <c r="C182" s="1">
+        <v>43232</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>234</v>
+      </c>
+      <c r="B185" t="s">
+        <v>164</v>
+      </c>
+      <c r="C185" s="1">
+        <v>43217</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>235</v>
+      </c>
+      <c r="B188" t="s">
+        <v>236</v>
+      </c>
+      <c r="C188" s="1">
+        <v>43201</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>237</v>
+      </c>
+      <c r="B191" t="s">
+        <v>238</v>
+      </c>
+      <c r="C191" s="1">
+        <v>43171</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>239</v>
+      </c>
+      <c r="B194" t="s">
+        <v>240</v>
+      </c>
+      <c r="C194" s="1">
+        <v>43165</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>241</v>
+      </c>
+      <c r="B197" t="s">
+        <v>129</v>
+      </c>
+      <c r="C197" s="1">
+        <v>43159</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>242</v>
+      </c>
+      <c r="B200" t="s">
+        <v>243</v>
+      </c>
+      <c r="C200" s="1">
+        <v>43135</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>244</v>
+      </c>
+      <c r="B203" t="s">
+        <v>245</v>
+      </c>
+      <c r="C203" s="1">
+        <v>43131</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>246</v>
+      </c>
+      <c r="B206" t="s">
+        <v>247</v>
+      </c>
+      <c r="C206" s="1">
+        <v>43125</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>248</v>
+      </c>
+      <c r="B209" t="s">
+        <v>249</v>
+      </c>
+      <c r="C209" s="1">
+        <v>43122</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>250</v>
+      </c>
+      <c r="B212" t="s">
+        <v>129</v>
+      </c>
+      <c r="C212" s="1">
+        <v>43122</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>251</v>
+      </c>
+      <c r="B215" t="s">
+        <v>252</v>
+      </c>
+      <c r="C215" s="1">
+        <v>43113</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>253</v>
+      </c>
+      <c r="B218" t="s">
+        <v>254</v>
+      </c>
+      <c r="C218" s="1">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>255</v>
+      </c>
+      <c r="B221" t="s">
+        <v>256</v>
+      </c>
+      <c r="C221" s="1">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>257</v>
+      </c>
+      <c r="B224" t="s">
+        <v>258</v>
+      </c>
+      <c r="C224" s="1">
+        <v>43103</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>259</v>
+      </c>
+      <c r="B227" t="s">
+        <v>122</v>
+      </c>
+      <c r="C227" s="1">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>260</v>
+      </c>
+      <c r="B230" t="s">
+        <v>261</v>
+      </c>
+      <c r="C230" s="1">
+        <v>43098</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>262</v>
+      </c>
+      <c r="B233" t="s">
+        <v>263</v>
+      </c>
+      <c r="C233" s="1">
+        <v>43098</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>264</v>
+      </c>
+      <c r="B236" t="s">
+        <v>265</v>
+      </c>
+      <c r="C236" s="1">
+        <v>43092</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>266</v>
+      </c>
+      <c r="B239" t="s">
+        <v>267</v>
+      </c>
+      <c r="C239" s="1">
+        <v>43083</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>268</v>
+      </c>
+      <c r="B242" t="s">
+        <v>269</v>
+      </c>
+      <c r="C242" s="1">
+        <v>43075</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>270</v>
+      </c>
+      <c r="B245" t="s">
+        <v>252</v>
+      </c>
+      <c r="C245" s="1">
+        <v>43073</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>271</v>
+      </c>
+      <c r="B248" t="s">
+        <v>252</v>
+      </c>
+      <c r="C248" s="1">
+        <v>43058</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>272</v>
+      </c>
+      <c r="B251" t="s">
+        <v>252</v>
+      </c>
+      <c r="C251" s="1">
+        <v>43058</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>273</v>
+      </c>
+      <c r="B254" t="s">
+        <v>240</v>
+      </c>
+      <c r="C254" s="1">
+        <v>43047</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>274</v>
+      </c>
+      <c r="B257" t="s">
+        <v>164</v>
+      </c>
+      <c r="C257" s="1">
+        <v>43039</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>275</v>
+      </c>
+      <c r="B260" t="s">
+        <v>252</v>
+      </c>
+      <c r="C260" s="1">
+        <v>43039</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>276</v>
+      </c>
+      <c r="B263" t="s">
+        <v>277</v>
+      </c>
+      <c r="C263" s="1">
+        <v>43005</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>278</v>
+      </c>
+      <c r="B266" t="s">
+        <v>279</v>
+      </c>
+      <c r="C266" s="1">
+        <v>42981</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>280</v>
+      </c>
+      <c r="B269" t="s">
+        <v>281</v>
+      </c>
+      <c r="C269" s="1">
+        <v>42977</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>282</v>
+      </c>
+      <c r="B272" t="s">
+        <v>283</v>
+      </c>
+      <c r="C272" s="1">
+        <v>42957</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>284</v>
+      </c>
+      <c r="B275" t="s">
+        <v>285</v>
+      </c>
+      <c r="C275" s="1">
+        <v>42954</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>286</v>
+      </c>
+      <c r="B278" t="s">
+        <v>287</v>
+      </c>
+      <c r="C278" s="1">
+        <v>42950</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>288</v>
+      </c>
+      <c r="B281" t="s">
+        <v>289</v>
+      </c>
+      <c r="C281" s="1">
+        <v>42945</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>290</v>
+      </c>
+      <c r="B284" t="s">
+        <v>291</v>
+      </c>
+      <c r="C284" s="1">
+        <v>42945</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>292</v>
+      </c>
+      <c r="B287" t="s">
+        <v>263</v>
+      </c>
+      <c r="C287" s="1">
+        <v>42941</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>293</v>
+      </c>
+      <c r="B290" t="s">
+        <v>294</v>
+      </c>
+      <c r="C290" s="1">
+        <v>42936</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>295</v>
+      </c>
+      <c r="B293" t="s">
+        <v>296</v>
+      </c>
+      <c r="C293" s="1">
+        <v>42898</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>297</v>
+      </c>
+      <c r="B296" t="s">
+        <v>298</v>
+      </c>
+      <c r="C296" s="1">
+        <v>42867</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>299</v>
+      </c>
+      <c r="B299" t="s">
+        <v>300</v>
+      </c>
+      <c r="C299" s="1">
+        <v>42819</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>301</v>
+      </c>
+      <c r="B302" t="s">
+        <v>302</v>
+      </c>
+      <c r="C302" s="1">
+        <v>42792</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>303</v>
+      </c>
+      <c r="B305" t="s">
+        <v>304</v>
+      </c>
+      <c r="C305" s="1">
+        <v>42781</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>305</v>
+      </c>
+      <c r="B308" t="s">
+        <v>306</v>
+      </c>
+      <c r="C308" s="1">
+        <v>42771</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>307</v>
+      </c>
+      <c r="B311" t="s">
+        <v>308</v>
+      </c>
+      <c r="C311" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>309</v>
+      </c>
+      <c r="B314" t="s">
+        <v>310</v>
+      </c>
+      <c r="C314" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>311</v>
+      </c>
+      <c r="B317" t="s">
+        <v>310</v>
+      </c>
+      <c r="C317" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>312</v>
+      </c>
+      <c r="B320" t="s">
+        <v>310</v>
+      </c>
+      <c r="C320" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>313</v>
+      </c>
+      <c r="B323" t="s">
+        <v>310</v>
+      </c>
+      <c r="C323" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>314</v>
+      </c>
+      <c r="B326" t="s">
+        <v>315</v>
+      </c>
+      <c r="C326" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>316</v>
+      </c>
+      <c r="B329" t="s">
+        <v>317</v>
+      </c>
+      <c r="C329" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>318</v>
+      </c>
+      <c r="B332" t="s">
+        <v>317</v>
+      </c>
+      <c r="C332" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>319</v>
+      </c>
+      <c r="B335" t="s">
+        <v>317</v>
+      </c>
+      <c r="C335" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>320</v>
+      </c>
+      <c r="B338" t="s">
+        <v>321</v>
+      </c>
+      <c r="C338" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>322</v>
+      </c>
+      <c r="B341" t="s">
+        <v>321</v>
+      </c>
+      <c r="C341" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>323</v>
+      </c>
+      <c r="B344" t="s">
+        <v>321</v>
+      </c>
+      <c r="C344" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>324</v>
+      </c>
+      <c r="B347" t="s">
+        <v>321</v>
+      </c>
+      <c r="C347" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>325</v>
+      </c>
+      <c r="B350" t="s">
+        <v>321</v>
+      </c>
+      <c r="C350" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>326</v>
+      </c>
+      <c r="B353" t="s">
+        <v>321</v>
+      </c>
+      <c r="C353" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>327</v>
+      </c>
+      <c r="B356" t="s">
+        <v>321</v>
+      </c>
+      <c r="C356" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>328</v>
+      </c>
+      <c r="B359" t="s">
+        <v>321</v>
+      </c>
+      <c r="C359" s="1">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>329</v>
+      </c>
+      <c r="B362" t="s">
+        <v>330</v>
+      </c>
+      <c r="C362" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>331</v>
+      </c>
+      <c r="B365" t="s">
+        <v>332</v>
+      </c>
+      <c r="C365" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>333</v>
+      </c>
+      <c r="B368" t="s">
+        <v>332</v>
+      </c>
+      <c r="C368" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>334</v>
+      </c>
+      <c r="B371" t="s">
+        <v>332</v>
+      </c>
+      <c r="C371" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>335</v>
+      </c>
+      <c r="B374" t="s">
+        <v>332</v>
+      </c>
+      <c r="C374" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>336</v>
+      </c>
+      <c r="B377" t="s">
+        <v>332</v>
+      </c>
+      <c r="C377" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>337</v>
+      </c>
+      <c r="B380" t="s">
+        <v>332</v>
+      </c>
+      <c r="C380" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>338</v>
+      </c>
+      <c r="B383" t="s">
+        <v>332</v>
+      </c>
+      <c r="C383" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>339</v>
+      </c>
+      <c r="B386" t="s">
+        <v>332</v>
+      </c>
+      <c r="C386" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>340</v>
+      </c>
+      <c r="B389" t="s">
+        <v>332</v>
+      </c>
+      <c r="C389" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>341</v>
+      </c>
+      <c r="B392" t="s">
+        <v>332</v>
+      </c>
+      <c r="C392" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>342</v>
+      </c>
+      <c r="B395" t="s">
+        <v>343</v>
+      </c>
+      <c r="C395" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>344</v>
+      </c>
+      <c r="B398" t="s">
+        <v>343</v>
+      </c>
+      <c r="C398" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>345</v>
+      </c>
+      <c r="B401" t="s">
+        <v>343</v>
+      </c>
+      <c r="C401" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>346</v>
+      </c>
+      <c r="B404" t="s">
+        <v>343</v>
+      </c>
+      <c r="C404" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>347</v>
+      </c>
+      <c r="B407" t="s">
+        <v>348</v>
+      </c>
+      <c r="C407" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>349</v>
+      </c>
+      <c r="B410" t="s">
+        <v>348</v>
+      </c>
+      <c r="C410" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>350</v>
+      </c>
+      <c r="B413" t="s">
+        <v>348</v>
+      </c>
+      <c r="C413" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>351</v>
+      </c>
+      <c r="B416" t="s">
+        <v>348</v>
+      </c>
+      <c r="C416" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>352</v>
+      </c>
+      <c r="B419" t="s">
+        <v>348</v>
+      </c>
+      <c r="C419" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>353</v>
+      </c>
+      <c r="B422" t="s">
+        <v>348</v>
+      </c>
+      <c r="C422" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>354</v>
+      </c>
+      <c r="B425" t="s">
+        <v>348</v>
+      </c>
+      <c r="C425" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>355</v>
+      </c>
+      <c r="B428" t="s">
+        <v>348</v>
+      </c>
+      <c r="C428" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>356</v>
+      </c>
+      <c r="B431" t="s">
+        <v>348</v>
+      </c>
+      <c r="C431" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>357</v>
+      </c>
+      <c r="B434" t="s">
+        <v>348</v>
+      </c>
+      <c r="C434" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>358</v>
+      </c>
+      <c r="B437" t="s">
+        <v>348</v>
+      </c>
+      <c r="C437" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>359</v>
+      </c>
+      <c r="B440" t="s">
+        <v>348</v>
+      </c>
+      <c r="C440" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>360</v>
+      </c>
+      <c r="B443" t="s">
+        <v>361</v>
+      </c>
+      <c r="C443" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>362</v>
+      </c>
+      <c r="B446" t="s">
+        <v>361</v>
+      </c>
+      <c r="C446" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>363</v>
+      </c>
+      <c r="B449" t="s">
+        <v>361</v>
+      </c>
+      <c r="C449" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>364</v>
+      </c>
+      <c r="B452" t="s">
+        <v>361</v>
+      </c>
+      <c r="C452" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>365</v>
+      </c>
+      <c r="B455" t="s">
+        <v>361</v>
+      </c>
+      <c r="C455" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>366</v>
+      </c>
+      <c r="B458" t="s">
+        <v>361</v>
+      </c>
+      <c r="C458" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>367</v>
+      </c>
+      <c r="B461" t="s">
+        <v>361</v>
+      </c>
+      <c r="C461" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>368</v>
+      </c>
+      <c r="B464" t="s">
+        <v>361</v>
+      </c>
+      <c r="C464" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>369</v>
+      </c>
+      <c r="B467" t="s">
+        <v>361</v>
+      </c>
+      <c r="C467" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>370</v>
+      </c>
+      <c r="B470" t="s">
+        <v>371</v>
+      </c>
+      <c r="C470" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>372</v>
+      </c>
+      <c r="B473" t="s">
+        <v>371</v>
+      </c>
+      <c r="C473" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>373</v>
+      </c>
+      <c r="B476" t="s">
+        <v>371</v>
+      </c>
+      <c r="C476" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>374</v>
+      </c>
+      <c r="B479" t="s">
+        <v>375</v>
+      </c>
+      <c r="C479" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>376</v>
+      </c>
+      <c r="B482" t="s">
+        <v>377</v>
+      </c>
+      <c r="C482" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>378</v>
+      </c>
+      <c r="B485" t="s">
+        <v>377</v>
+      </c>
+      <c r="C485" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>379</v>
+      </c>
+      <c r="B488" t="s">
+        <v>380</v>
+      </c>
+      <c r="C488" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>381</v>
+      </c>
+      <c r="B491" t="s">
+        <v>382</v>
+      </c>
+      <c r="C491" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>383</v>
+      </c>
+      <c r="B494" t="s">
+        <v>384</v>
+      </c>
+      <c r="C494" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>385</v>
+      </c>
+      <c r="B497" t="s">
+        <v>386</v>
+      </c>
+      <c r="C497" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>387</v>
+      </c>
+      <c r="B500" t="s">
+        <v>298</v>
+      </c>
+      <c r="C500" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>388</v>
+      </c>
+      <c r="B503" t="s">
+        <v>389</v>
+      </c>
+      <c r="C503" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>390</v>
+      </c>
+      <c r="B506" t="s">
+        <v>391</v>
+      </c>
+      <c r="C506" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>392</v>
+      </c>
+      <c r="B509" t="s">
+        <v>393</v>
+      </c>
+      <c r="C509" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>394</v>
+      </c>
+      <c r="B512" t="s">
+        <v>395</v>
+      </c>
+      <c r="C512" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>396</v>
+      </c>
+      <c r="B515" t="s">
+        <v>397</v>
+      </c>
+      <c r="C515" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>398</v>
+      </c>
+      <c r="B518" t="s">
+        <v>399</v>
+      </c>
+      <c r="C518" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>400</v>
+      </c>
+      <c r="B521" t="s">
+        <v>298</v>
+      </c>
+      <c r="C521" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>401</v>
+      </c>
+      <c r="B524" t="s">
+        <v>298</v>
+      </c>
+      <c r="C524" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>402</v>
+      </c>
+      <c r="B527" t="s">
+        <v>298</v>
+      </c>
+      <c r="C527" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>403</v>
+      </c>
+      <c r="B530" t="s">
+        <v>298</v>
+      </c>
+      <c r="C530" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>404</v>
+      </c>
+      <c r="B533" t="s">
+        <v>405</v>
+      </c>
+      <c r="C533" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>406</v>
+      </c>
+      <c r="B536" t="s">
+        <v>407</v>
+      </c>
+      <c r="C536" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="539" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
+        <v>408</v>
+      </c>
+      <c r="B539" t="s">
+        <v>409</v>
+      </c>
+      <c r="C539" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="542" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>410</v>
+      </c>
+      <c r="B542" t="s">
+        <v>411</v>
+      </c>
+      <c r="C542" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="545" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>412</v>
+      </c>
+      <c r="B545" t="s">
+        <v>411</v>
+      </c>
+      <c r="C545" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>413</v>
+      </c>
+      <c r="B548" t="s">
+        <v>414</v>
+      </c>
+      <c r="C548" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="551" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>415</v>
+      </c>
+      <c r="B551" t="s">
+        <v>416</v>
+      </c>
+      <c r="C551" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="554" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>417</v>
+      </c>
+      <c r="B554" t="s">
+        <v>418</v>
+      </c>
+      <c r="C554" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="557" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>419</v>
+      </c>
+      <c r="B557" t="s">
+        <v>420</v>
+      </c>
+      <c r="C557" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="560" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>421</v>
+      </c>
+      <c r="B560" t="s">
+        <v>422</v>
+      </c>
+      <c r="C560" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="563" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>423</v>
+      </c>
+      <c r="B563" t="s">
+        <v>422</v>
+      </c>
+      <c r="C563" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>424</v>
+      </c>
+      <c r="B566" t="s">
+        <v>425</v>
+      </c>
+      <c r="C566" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>426</v>
+      </c>
+      <c r="B569" t="s">
+        <v>427</v>
+      </c>
+      <c r="C569" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="572" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>428</v>
+      </c>
+      <c r="B572" t="s">
+        <v>429</v>
+      </c>
+      <c r="C572" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="575" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>430</v>
+      </c>
+      <c r="B575" t="s">
+        <v>261</v>
+      </c>
+      <c r="C575" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="578" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A578">
+        <v>1984</v>
+      </c>
+      <c r="B578" t="s">
+        <v>431</v>
+      </c>
+      <c r="C578" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="581" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>432</v>
+      </c>
+      <c r="B581" t="s">
+        <v>433</v>
+      </c>
+      <c r="C581" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="584" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>434</v>
+      </c>
+      <c r="B584" t="s">
+        <v>435</v>
+      </c>
+      <c r="C584" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="587" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>436</v>
+      </c>
+      <c r="B587" t="s">
+        <v>377</v>
+      </c>
+      <c r="C587" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="590" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>437</v>
+      </c>
+      <c r="B590" t="s">
+        <v>438</v>
+      </c>
+      <c r="C590" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="593" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>439</v>
+      </c>
+      <c r="B593" t="s">
+        <v>440</v>
+      </c>
+      <c r="C593" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="596" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>441</v>
+      </c>
+      <c r="B596" t="s">
+        <v>442</v>
+      </c>
+      <c r="C596" s="1">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="599" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>443</v>
+      </c>
+      <c r="B599" t="s">
+        <v>444</v>
+      </c>
+      <c r="C599" s="1">
+        <v>42737</v>
+      </c>
+    </row>
+    <row r="602" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>445</v>
+      </c>
+      <c r="B602" t="s">
+        <v>446</v>
+      </c>
+      <c r="C602" s="1">
+        <v>42559</v>
+      </c>
+    </row>
+    <row r="605" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>447</v>
+      </c>
+      <c r="B605" t="s">
+        <v>448</v>
+      </c>
+      <c r="C605" s="1">
+        <v>42559</v>
+      </c>
+    </row>
+    <row r="608" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>449</v>
+      </c>
+      <c r="B608" t="s">
+        <v>450</v>
+      </c>
+      <c r="C608" s="1">
+        <v>42559</v>
+      </c>
+    </row>
+    <row r="611" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
+        <v>451</v>
+      </c>
+      <c r="B611" t="s">
+        <v>433</v>
+      </c>
+      <c r="C611" s="1">
+        <v>42559</v>
+      </c>
+    </row>
+    <row r="614" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>452</v>
+      </c>
+      <c r="B614" t="s">
+        <v>411</v>
+      </c>
+      <c r="C614" s="1">
+        <v>42551</v>
+      </c>
+    </row>
+    <row r="617" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A617" t="s">
+        <v>453</v>
+      </c>
+      <c r="B617" t="s">
+        <v>454</v>
+      </c>
+      <c r="C617" s="1">
+        <v>42551</v>
+      </c>
+    </row>
+    <row r="620" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A620" t="s">
+        <v>455</v>
+      </c>
+      <c r="B620" t="s">
+        <v>456</v>
+      </c>
+      <c r="C620" s="1">
+        <v>42548</v>
+      </c>
+    </row>
+    <row r="623" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>457</v>
+      </c>
+      <c r="B623" t="s">
+        <v>238</v>
+      </c>
+      <c r="C623" s="1">
+        <v>42548</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A626" t="s">
+        <v>458</v>
+      </c>
+      <c r="B626" t="s">
+        <v>459</v>
+      </c>
+      <c r="C626" s="1">
+        <v>42548</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>